<commit_message>
versión inicial HiveSim online
</commit_message>
<xml_diff>
--- a/Data/2025/10_October/2025-10-21_promedios.xlsx
+++ b/Data/2025/10_October/2025-10-21_promedios.xlsx
@@ -30,7 +30,7 @@
       <color rgb="00000000"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -47,6 +47,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00FFF2CC"/>
         <bgColor rgb="00FFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F8CBAD"/>
+        <bgColor rgb="00F8CBAD"/>
       </patternFill>
     </fill>
   </fills>
@@ -76,12 +82,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -447,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,7 +471,7 @@
     <col width="21" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="8" max="8"/>
     <col width="16" customWidth="1" min="9" max="9"/>
-    <col width="78" customWidth="1" min="10" max="10"/>
+    <col width="117" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -871,6 +878,270 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>2025-10-21</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>14:12:17</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>26.13</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>42.8</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>20.76</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="G10" s="3" t="inlineStr">
+        <is>
+          <t>cielo claro</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>Crítica</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>Precaución</t>
+        </is>
+      </c>
+      <c r="J10" s="3" t="inlineStr">
+        <is>
+          <t>🚨 Temperatura crítica (26.1 °C; fuera del rango 30–38 °C). ⚠️ Humedad fuera del rango óptimo (42.8%; ideal 50–75%).</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>2025-10-21</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>14:23:05</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>26.16</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>42.23</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>20.76</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="G11" s="3" t="inlineStr">
+        <is>
+          <t>cielo claro</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>Crítica</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>Precaución</t>
+        </is>
+      </c>
+      <c r="J11" s="3" t="inlineStr">
+        <is>
+          <t>🚨 Temperatura crítica (26.2 °C; fuera del rango 30–38 °C). ⚠️ Humedad fuera del rango óptimo (42.2%; ideal 50–75%).</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>2025-10-21</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>14:33:50</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>26.17</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>41.52</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>21.13</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="G12" s="3" t="inlineStr">
+        <is>
+          <t>cielo claro</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>Crítica</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>Precaución</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>🚨 Temperatura crítica (26.2 °C; fuera del rango 30–38 °C). ⚠️ Humedad fuera del rango óptimo (41.5%; ideal 50–75%).</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>2025-10-21</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>14:44:34</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>26.33</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>42.2</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>21.13</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="G13" s="3" t="inlineStr">
+        <is>
+          <t>cielo claro</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>Crítica</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>Precaución</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
+        <is>
+          <t>🚨 Temperatura crítica (26.3 °C; fuera del rango 30–38 °C). ⚠️ Humedad fuera del rango óptimo (42.2%; ideal 50–75%).</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>2025-10-21</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>14:55:22</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>26.37</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>41.47</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>21.13</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="G14" s="3" t="inlineStr">
+        <is>
+          <t>cielo claro</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>Crítica</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>Precaución</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>🚨 Temperatura crítica (26.4 °C; fuera del rango 30–38 °C). ⚠️ Humedad fuera del rango óptimo (41.5%; ideal 50–75%).</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>2025-10-21</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>15:06:09</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>26.37</v>
+      </c>
+      <c r="D15" s="3" t="n">
+        <v>41.57</v>
+      </c>
+      <c r="E15" s="3" t="n">
+        <v>21.13</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
+          <t>cielo claro</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>Crítica</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>Precaución</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>🚨 Temperatura crítica (26.4 °C; fuera del rango 30–38 °C). ⚠️ Humedad fuera del rango óptimo (41.6%; ideal 50–75%).</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>